<commit_message>
TL S40001, Re-TL S40000
</commit_message>
<xml_diff>
--- a/tl/S40000.MES.BIN.xlsx
+++ b/tl/S40000.MES.BIN.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6F8ACB-6AB6-4BD5-8C19-AE7E43864819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E96C8A-5329-424D-B84D-0302E990EDFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6240" yWindow="6240" windowWidth="49560" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3045" yWindow="15825" windowWidth="49560" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S40000.MES.BIN" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="182">
   <si>
     <t>Status</t>
   </si>
@@ -206,13 +206,16 @@
     <t>43</t>
   </si>
   <si>
+    <t>So Akira knew Misaki was here...</t>
+  </si>
+  <si>
     <t>I can't believe Akira knew that Misaki-san was here...</t>
   </si>
   <si>
     <t>45</t>
   </si>
   <si>
-    <t>And, when I look at him, he has a genuinely surprised look on his face.</t>
+    <t>When I look at him, he has a genuinely surprised look on his face.</t>
   </si>
   <si>
     <t>47</t>
@@ -236,18 +239,24 @@
     <t>53</t>
   </si>
   <si>
+    <t>Now that I think about it, is Nanase-kun too?</t>
+  </si>
+  <si>
     <t>Come to think of it, is Nanase-kun too?</t>
   </si>
   <si>
     <t>55</t>
   </si>
   <si>
-    <t>We're on our way back now, but...</t>
+    <t>We're on our way home now, but...</t>
   </si>
   <si>
     <t>57</t>
   </si>
   <si>
+    <t>Ah, that's right.</t>
+  </si>
+  <si>
     <t>Oh, right.</t>
   </si>
   <si>
@@ -287,27 +296,33 @@
     <t>69</t>
   </si>
   <si>
+    <t>But today is different.</t>
+  </si>
+  <si>
     <t>But today of all days, it's like this.</t>
   </si>
   <si>
     <t>71</t>
   </si>
   <si>
-    <t>Ah-... I messed up...</t>
-  </si>
-  <si>
     <t>Ah-... I failed...</t>
   </si>
   <si>
     <t>73</t>
   </si>
   <si>
+    <t>Can't you just buy the magazine?</t>
+  </si>
+  <si>
     <t>Why don't you just buy the magazine?</t>
   </si>
   <si>
     <t>75</t>
   </si>
   <si>
+    <t>But it's expensive. And if it's a special that features an author I don't like, wouldn't it be a waste?</t>
+  </si>
+  <si>
     <t>Because it's expensive. And if it's a special that features an author I don't like, I wouldn't want it, would I?</t>
   </si>
   <si>
@@ -320,7 +335,7 @@
     <t>79</t>
   </si>
   <si>
-    <t>That's how it is.</t>
+    <t>That's just how it is.</t>
   </si>
   <si>
     <t>81</t>
@@ -332,7 +347,7 @@
     <t>83</t>
   </si>
   <si>
-    <t>It's my fault for forgetting. Let's do it tomorrow.</t>
+    <t>It's your fault for forgetting. Let's do it tomorrow.</t>
   </si>
   <si>
     <t>85</t>
@@ -362,7 +377,7 @@
     <t>93</t>
   </si>
   <si>
-    <t>I also mention that we forgot that a new book was arriving at the library (while trying to make it sound interesting).</t>
+    <t>I also mention that he forgot that new books were arriving at the library (while trying to make it sound interesting).</t>
   </si>
   <si>
     <t>95</t>
@@ -374,9 +389,15 @@
     <t>97</t>
   </si>
   <si>
+    <t>Wasn't there a special on Gardner this month? (Gardner is a lawyer and author)</t>
+  </si>
+  <si>
     <t>Wasn't there a feature on a guy named Gardner this month?</t>
   </si>
   <si>
+    <t>Deliberately add context</t>
+  </si>
+  <si>
     <t>99</t>
   </si>
   <si>
@@ -386,6 +407,9 @@
     <t>101</t>
   </si>
   <si>
+    <t>Wasn't he the guy who created the fictional defense attorney, Perry Mason?</t>
+  </si>
+  <si>
     <t>Wasn't he the guy from Perry Mason?</t>
   </si>
   <si>
@@ -398,7 +422,10 @@
     <t>105</t>
   </si>
   <si>
-    <t>I see. Damn. Good thing in the midst of misfortune...?</t>
+    <t>I see. Fufu. Good thing in the midst of misfortune...?</t>
+  </si>
+  <si>
+    <t>くすっ is a giggle.</t>
   </si>
   <si>
     <t>107</t>
@@ -425,10 +452,7 @@
     <t>113</t>
   </si>
   <si>
-    <t>Akira just laughs simply. He really is a man of small happiness.</t>
-  </si>
-  <si>
-    <t>This is awkward... With row 56</t>
+    <t>Akira just laughs simply. He really is a small happiness man.</t>
   </si>
   <si>
     <t>115</t>
@@ -446,12 +470,18 @@
     <t>119</t>
   </si>
   <si>
+    <t>...Well, never mind.</t>
+  </si>
+  <si>
     <t>Well, it's okay.</t>
   </si>
   <si>
     <t>121</t>
   </si>
   <si>
+    <t>That's why, you see, Akira, you better hurry or you'll be late.</t>
+  </si>
+  <si>
     <t>That's why, look, Akira, you better hurry or you'll be late.</t>
   </si>
   <si>
@@ -476,6 +506,9 @@
     <t>129</t>
   </si>
   <si>
+    <t>I didn't, I didn't. Well, I can hang out and then go home though.</t>
+  </si>
+  <si>
     <t>I'm not, I'm not. Well, I can stay to hang out and then go home.</t>
   </si>
   <si>
@@ -488,7 +521,10 @@
     <t>133</t>
   </si>
   <si>
-    <t>Damn... Fujii-kun...</t>
+    <t>Fufu... Fujii-kun...</t>
+  </si>
+  <si>
+    <t>くすっ is a giggle</t>
   </si>
   <si>
     <t>135</t>
@@ -518,7 +554,7 @@
     <t>143</t>
   </si>
   <si>
-    <t>Go with Misaki to the library.</t>
+    <t>Go with Misaki-san to the library.</t>
   </si>
   <si>
     <t>145</t>
@@ -947,7 +983,7 @@
   <dimension ref="A1:J74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1679,10 +1715,10 @@
         <v>9</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>9</v>
@@ -1699,7 +1735,7 @@
         <v>9</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>9</v>
@@ -1714,7 +1750,7 @@
         <v>9</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>9</v>
@@ -1731,7 +1767,7 @@
         <v>9</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
@@ -1746,7 +1782,7 @@
         <v>9</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H25" s="5" t="s">
         <v>9</v>
@@ -1763,7 +1799,7 @@
         <v>9</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>10</v>
@@ -1778,7 +1814,7 @@
         <v>9</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>9</v>
@@ -1795,7 +1831,7 @@
         <v>9</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>59</v>
@@ -1810,7 +1846,7 @@
         <v>9</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>9</v>
@@ -1827,7 +1863,7 @@
         <v>9</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>59</v>
@@ -1839,10 +1875,10 @@
         <v>9</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>9</v>
@@ -1859,7 +1895,7 @@
         <v>9</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>10</v>
@@ -1874,7 +1910,7 @@
         <v>9</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>9</v>
@@ -1891,7 +1927,7 @@
         <v>9</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>9</v>
@@ -1903,10 +1939,10 @@
         <v>9</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>9</v>
@@ -1923,7 +1959,7 @@
         <v>9</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>9</v>
@@ -1938,7 +1974,7 @@
         <v>9</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>9</v>
@@ -1955,7 +1991,7 @@
         <v>9</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>9</v>
@@ -1970,7 +2006,7 @@
         <v>9</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>9</v>
@@ -1987,7 +2023,7 @@
         <v>9</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>10</v>
@@ -1999,10 +2035,10 @@
         <v>9</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>9</v>
@@ -2019,7 +2055,7 @@
         <v>9</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>9</v>
@@ -2034,7 +2070,7 @@
         <v>9</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>9</v>
@@ -2051,7 +2087,7 @@
         <v>9</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>9</v>
@@ -2066,7 +2102,7 @@
         <v>9</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>9</v>
@@ -2083,7 +2119,7 @@
         <v>9</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>9</v>
@@ -2095,10 +2131,10 @@
         <v>9</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>9</v>
+        <v>93</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>9</v>
@@ -2115,7 +2151,7 @@
         <v>9</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>9</v>
@@ -2127,10 +2163,10 @@
         <v>9</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>9</v>
@@ -2147,7 +2183,7 @@
         <v>9</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>10</v>
@@ -2159,10 +2195,10 @@
         <v>9</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>9</v>
+        <v>98</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="H38" s="3" t="s">
         <v>9</v>
@@ -2179,7 +2215,7 @@
         <v>9</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>9</v>
@@ -2191,10 +2227,10 @@
         <v>9</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>9</v>
+        <v>101</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>9</v>
@@ -2211,7 +2247,7 @@
         <v>9</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>10</v>
@@ -2226,7 +2262,7 @@
         <v>9</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="H40" s="3" t="s">
         <v>9</v>
@@ -2243,7 +2279,7 @@
         <v>9</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>9</v>
@@ -2258,7 +2294,7 @@
         <v>9</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>9</v>
@@ -2275,7 +2311,7 @@
         <v>9</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>9</v>
@@ -2290,7 +2326,7 @@
         <v>9</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>9</v>
@@ -2307,7 +2343,7 @@
         <v>9</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>10</v>
@@ -2322,7 +2358,7 @@
         <v>9</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>9</v>
@@ -2339,7 +2375,7 @@
         <v>9</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>9</v>
@@ -2354,7 +2390,7 @@
         <v>9</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="H44" s="3" t="s">
         <v>9</v>
@@ -2371,7 +2407,7 @@
         <v>9</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>59</v>
@@ -2386,7 +2422,7 @@
         <v>9</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="H45" s="5" t="s">
         <v>9</v>
@@ -2403,7 +2439,7 @@
         <v>9</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>9</v>
@@ -2418,7 +2454,7 @@
         <v>9</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="H46" s="3" t="s">
         <v>9</v>
@@ -2435,7 +2471,7 @@
         <v>9</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>9</v>
@@ -2450,7 +2486,7 @@
         <v>9</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>9</v>
@@ -2467,7 +2503,7 @@
         <v>9</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>9</v>
@@ -2482,7 +2518,7 @@
         <v>9</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="H48" s="3" t="s">
         <v>9</v>
@@ -2499,7 +2535,7 @@
         <v>9</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>59</v>
@@ -2514,7 +2550,7 @@
         <v>9</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="H49" s="5" t="s">
         <v>9</v>
@@ -2531,7 +2567,7 @@
         <v>9</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>59</v>
@@ -2543,13 +2579,13 @@
         <v>9</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>9</v>
+        <v>124</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>9</v>
+        <v>126</v>
       </c>
       <c r="I50" s="3" t="s">
         <v>9</v>
@@ -2563,7 +2599,7 @@
         <v>9</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>9</v>
@@ -2578,7 +2614,7 @@
         <v>9</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="H51" s="5" t="s">
         <v>9</v>
@@ -2595,7 +2631,7 @@
         <v>9</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>59</v>
@@ -2607,13 +2643,13 @@
         <v>9</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>9</v>
+        <v>130</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>9</v>
+        <v>126</v>
       </c>
       <c r="I52" s="3" t="s">
         <v>9</v>
@@ -2627,7 +2663,7 @@
         <v>9</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>9</v>
@@ -2642,7 +2678,7 @@
         <v>9</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="H53" s="5" t="s">
         <v>9</v>
@@ -2659,7 +2695,7 @@
         <v>9</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>59</v>
@@ -2674,10 +2710,10 @@
         <v>9</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>9</v>
+        <v>136</v>
       </c>
       <c r="I54" s="3" t="s">
         <v>9</v>
@@ -2691,7 +2727,7 @@
         <v>9</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>9</v>
@@ -2706,7 +2742,7 @@
         <v>9</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="H55" s="5" t="s">
         <v>9</v>
@@ -2723,7 +2759,7 @@
         <v>9</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>9</v>
@@ -2735,10 +2771,10 @@
         <v>9</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="H56" s="3" t="s">
         <v>9</v>
@@ -2755,7 +2791,7 @@
         <v>9</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>9</v>
@@ -2770,7 +2806,7 @@
         <v>9</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="H57" s="5" t="s">
         <v>9</v>
@@ -2787,7 +2823,7 @@
         <v>9</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>9</v>
@@ -2802,10 +2838,10 @@
         <v>9</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>137</v>
+        <v>9</v>
       </c>
       <c r="I58" s="3" t="s">
         <v>9</v>
@@ -2819,7 +2855,7 @@
         <v>9</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>9</v>
@@ -2834,7 +2870,7 @@
         <v>9</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="H59" s="5" t="s">
         <v>9</v>
@@ -2851,7 +2887,7 @@
         <v>9</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>9</v>
@@ -2866,7 +2902,7 @@
         <v>9</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="H60" s="3" t="s">
         <v>9</v>
@@ -2883,7 +2919,7 @@
         <v>9</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>9</v>
@@ -2895,10 +2931,10 @@
         <v>9</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>9</v>
+        <v>151</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="H61" s="5" t="s">
         <v>9</v>
@@ -2915,7 +2951,7 @@
         <v>9</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>10</v>
@@ -2927,10 +2963,10 @@
         <v>9</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>9</v>
+        <v>154</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="H62" s="3" t="s">
         <v>9</v>
@@ -2947,7 +2983,7 @@
         <v>9</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>9</v>
@@ -2962,7 +2998,7 @@
         <v>9</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="H63" s="5" t="s">
         <v>9</v>
@@ -2979,7 +3015,7 @@
         <v>9</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>10</v>
@@ -2994,7 +3030,7 @@
         <v>9</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="H64" s="3" t="s">
         <v>9</v>
@@ -3011,7 +3047,7 @@
         <v>9</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>9</v>
@@ -3026,7 +3062,7 @@
         <v>9</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="H65" s="5" t="s">
         <v>9</v>
@@ -3043,7 +3079,7 @@
         <v>9</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>10</v>
@@ -3055,10 +3091,10 @@
         <v>9</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>9</v>
+        <v>163</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="H66" s="3" t="s">
         <v>9</v>
@@ -3075,7 +3111,7 @@
         <v>9</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>9</v>
@@ -3090,7 +3126,7 @@
         <v>9</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="H67" s="5" t="s">
         <v>9</v>
@@ -3107,7 +3143,7 @@
         <v>9</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>59</v>
@@ -3122,10 +3158,10 @@
         <v>9</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>9</v>
+        <v>169</v>
       </c>
       <c r="I68" s="3" t="s">
         <v>9</v>
@@ -3139,7 +3175,7 @@
         <v>9</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>9</v>
@@ -3154,7 +3190,7 @@
         <v>9</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="H69" s="5" t="s">
         <v>9</v>
@@ -3171,7 +3207,7 @@
         <v>9</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>59</v>
@@ -3186,7 +3222,7 @@
         <v>9</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="H70" s="3" t="s">
         <v>9</v>
@@ -3203,7 +3239,7 @@
         <v>9</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>162</v>
+        <v>174</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>9</v>
@@ -3218,7 +3254,7 @@
         <v>9</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="H71" s="5" t="s">
         <v>9</v>
@@ -3235,7 +3271,7 @@
         <v>9</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>9</v>
@@ -3250,7 +3286,7 @@
         <v>9</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="H72" s="3" t="s">
         <v>9</v>
@@ -3267,7 +3303,7 @@
         <v>9</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>9</v>
@@ -3282,7 +3318,7 @@
         <v>9</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="H73" s="5" t="s">
         <v>9</v>
@@ -3299,7 +3335,7 @@
         <v>9</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>9</v>
@@ -3314,7 +3350,7 @@
         <v>9</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>169</v>
+        <v>181</v>
       </c>
       <c r="H74" s="3" t="s">
         <v>9</v>

</xml_diff>